<commit_message>
Adding IQC, ASH, new customer
</commit_message>
<xml_diff>
--- a/dictionary/customer_name.xlsx
+++ b/dictionary/customer_name.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/R project/CMML_report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Documents/GitHub/CMML/dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4CA1BD-8CF0-644F-9787-02CB1E910D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2719F198-2DB5-8B43-9F48-BBE819FE5F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="1540" windowWidth="21360" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7400" yWindow="500" windowWidth="21360" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>customer_name</t>
   </si>
@@ -42,18 +42,9 @@
     <t>Sunrise Hospital</t>
   </si>
   <si>
-    <t>Central Media Making Laboratory</t>
-  </si>
-  <si>
     <t>Kossamak</t>
   </si>
   <si>
-    <t>Sihanouk Hospital Center of Hope</t>
-  </si>
-  <si>
-    <t>Khmer Soviet Friendship Hospital</t>
-  </si>
-  <si>
     <t>Takeo</t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t>Pro Labpratory</t>
   </si>
   <si>
-    <t>Diagnostic and Detection Laboratory</t>
-  </si>
-  <si>
     <t>Svay Rieng</t>
   </si>
   <si>
@@ -127,6 +115,21 @@
   </si>
   <si>
     <t>Royal Phnom Penh hospital</t>
+  </si>
+  <si>
+    <t>DDL</t>
+  </si>
+  <si>
+    <t>CMML</t>
+  </si>
+  <si>
+    <t>KSFH</t>
+  </si>
+  <si>
+    <t>SHCH</t>
+  </si>
+  <si>
+    <t>Gold Medical Diagnostic Laboratory</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="137" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="137" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -510,10 +513,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -548,7 +551,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3">
         <v>104.906479</v>
@@ -563,7 +566,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3">
         <v>104.890378</v>
@@ -578,7 +581,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3">
         <v>104.924514</v>
@@ -593,7 +596,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3">
         <v>104.90398399999999</v>
@@ -608,7 +611,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
         <v>104.782827</v>
@@ -623,7 +626,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>104.903887</v>
@@ -638,7 +641,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3">
         <v>104.89872200000001</v>
@@ -653,7 +656,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3">
         <v>103.201818</v>
@@ -668,7 +671,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3">
         <v>104.916698</v>
@@ -683,7 +686,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3">
         <v>104.899123</v>
@@ -698,7 +701,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3">
         <v>104.881167</v>
@@ -713,7 +716,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>104.89724099999999</v>
@@ -728,7 +731,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3">
         <v>104.91499399999999</v>
@@ -743,7 +746,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3">
         <v>104.898168</v>
@@ -758,7 +761,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3">
         <v>105.459999</v>
@@ -773,7 +776,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
         <v>104.926411</v>
@@ -788,7 +791,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3">
         <v>104.892213</v>
@@ -803,7 +806,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3">
         <v>104.921887</v>
@@ -818,7 +821,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B22" s="3">
         <v>104.923551</v>
@@ -833,7 +836,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3">
         <v>105.802159</v>
@@ -848,13 +851,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3">
-        <v>104.13202</v>
+        <v>104.132008743602</v>
       </c>
       <c r="C24">
-        <v>10.570066000000001</v>
+        <v>10.570141163026801</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="3"/>
@@ -863,7 +866,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B25" s="3">
         <v>104.922612</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" s="3">
         <v>104.922798</v>
@@ -893,7 +896,7 @@
     </row>
     <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3">
         <v>104.880652</v>
@@ -908,7 +911,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28" s="3">
         <v>103.201818</v>
@@ -923,7 +926,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B29" s="3">
         <v>104.901325</v>
@@ -938,7 +941,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B30" s="3">
         <v>104.914193</v>
@@ -950,6 +953,17 @@
       <c r="G30" s="3"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="3">
+        <v>104.926276</v>
+      </c>
+      <c r="C31">
+        <v>11.572371</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>